<commit_message>
Started work on results.
</commit_message>
<xml_diff>
--- a/graphics_generation/elisa/tecan/elisa_anti_pvx_15_min.xlsx
+++ b/graphics_generation/elisa/tecan/elisa_anti_pvx_15_min.xlsx
@@ -161,13 +161,13 @@
     <t>Datum:</t>
   </si>
   <si>
-    <t>26.06.2025</t>
+    <t>30.06.2025</t>
   </si>
   <si>
     <t>Zeit:</t>
   </si>
   <si>
-    <t>14:58:18</t>
+    <t>14:08:07</t>
   </si>
   <si>
     <t>System</t>
@@ -233,16 +233,16 @@
     <t>Bereich der Platte</t>
   </si>
   <si>
-    <t>B1-G12</t>
+    <t>B2-G11</t>
   </si>
   <si>
     <t>Startzeit:</t>
   </si>
   <si>
-    <t>26.06.2025 14:58:23</t>
-  </si>
-  <si>
-    <t>Temperatur: 24.5 °C</t>
+    <t>30.06.2025 14:08:12</t>
+  </si>
+  <si>
+    <t>Temperatur: 26.6 °C</t>
   </si>
   <si>
     <t>&lt;&gt;</t>
@@ -269,7 +269,7 @@
     <t>Endzeit:</t>
   </si>
   <si>
-    <t>26.06.2025 14:59:23</t>
+    <t>30.06.2025 14:09:02</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
@@ -845,12 +845,12 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -858,7 +858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -869,7 +869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -880,7 +880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -888,7 +888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -899,7 +899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -907,7 +907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -915,299 +915,257 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E28" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F28" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G28" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H28" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I28" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J28" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K28" s="3">
-        <v>10</v>
-      </c>
-      <c r="L28" s="3">
         <v>11</v>
       </c>
-      <c r="M28" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B29">
-        <v>0.13930000364780426</v>
+        <v>0.3513999879360199</v>
       </c>
       <c r="C29">
-        <v>0.10729999840259552</v>
+        <v>0.33539998531341553</v>
       </c>
       <c r="D29">
-        <v>0.1103999987244606</v>
+        <v>0.32499998807907104</v>
       </c>
       <c r="E29">
-        <v>9.0400002896785736E-2</v>
+        <v>0.98430001735687256</v>
       </c>
       <c r="F29">
-        <v>9.3099996447563171E-2</v>
+        <v>1.0124000310897827</v>
       </c>
       <c r="G29">
-        <v>9.3000002205371857E-2</v>
+        <v>1.0039999485015869</v>
       </c>
       <c r="H29">
-        <v>8.9400000870227814E-2</v>
+        <v>1.4298000335693359</v>
       </c>
       <c r="I29">
-        <v>9.0499997138977051E-2</v>
+        <v>1.4312000274658203</v>
       </c>
       <c r="J29">
-        <v>9.3599997460842133E-2</v>
+        <v>1.4364999532699585</v>
       </c>
       <c r="K29">
-        <v>0.12710000574588776</v>
-      </c>
-      <c r="L29">
-        <v>0.13570000231266022</v>
-      </c>
-      <c r="M29">
-        <v>0.16259999573230743</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.13330000638961792</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B30">
-        <v>0.11879999935626984</v>
+        <v>0.30579999089241028</v>
       </c>
       <c r="C30">
-        <v>0.10170000046491623</v>
+        <v>0.35210001468658447</v>
       </c>
       <c r="D30">
-        <v>0.10209999978542328</v>
+        <v>0.3294999897480011</v>
       </c>
       <c r="E30">
-        <v>8.8500000536441803E-2</v>
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>9.2399999499320984E-2</v>
+        <v>1.0078999996185303</v>
       </c>
       <c r="G30">
-        <v>8.3300001919269562E-2</v>
+        <v>0.99910002946853638</v>
       </c>
       <c r="H30">
-        <v>9.0700000524520874E-2</v>
+        <v>1.1679999828338623</v>
       </c>
       <c r="I30">
-        <v>8.9299999177455902E-2</v>
+        <v>1.1233999729156494</v>
       </c>
       <c r="J30">
-        <v>9.08999964594841E-2</v>
+        <v>1.1060999631881714</v>
       </c>
       <c r="K30">
-        <v>0.11509999632835388</v>
-      </c>
-      <c r="L30">
-        <v>0.11749999970197678</v>
-      </c>
-      <c r="M30">
-        <v>0.12559999525547028</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.18359999358654022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B31">
-        <v>0.11050000041723251</v>
+        <v>0.34670001268386841</v>
       </c>
       <c r="C31">
-        <v>9.5600001513957977E-2</v>
+        <v>0.3919999897480011</v>
       </c>
       <c r="D31">
-        <v>9.5700003206729889E-2</v>
+        <v>0.35069999098777771</v>
       </c>
       <c r="E31">
-        <v>8.8399998843669891E-2</v>
+        <v>0.13750000298023224</v>
       </c>
       <c r="F31">
-        <v>8.6099997162818909E-2</v>
+        <v>0.17990000545978546</v>
       </c>
       <c r="G31">
-        <v>8.8899999856948853E-2</v>
+        <v>0.17730000615119934</v>
       </c>
       <c r="H31">
-        <v>8.6800001561641693E-2</v>
+        <v>0.73189997673034668</v>
       </c>
       <c r="I31">
-        <v>8.829999715089798E-2</v>
+        <v>0.70389997959136963</v>
       </c>
       <c r="J31">
-        <v>8.8799998164176941E-2</v>
+        <v>0.74239999055862427</v>
       </c>
       <c r="K31">
-        <v>0.10010000318288803</v>
-      </c>
-      <c r="L31">
-        <v>0.10090000182390213</v>
-      </c>
-      <c r="M31">
-        <v>0.10490000247955322</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.11129999905824661</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B32">
-        <v>0.12110000103712082</v>
+        <v>0.34509998559951782</v>
       </c>
       <c r="C32">
-        <v>0.10490000247955322</v>
+        <v>0.3513999879360199</v>
       </c>
       <c r="D32">
-        <v>0.10130000114440918</v>
+        <v>0.34209999442100525</v>
       </c>
       <c r="E32">
-        <v>0.16509999334812164</v>
+        <v>0.10329999774694443</v>
       </c>
       <c r="F32">
-        <v>0.16820000112056732</v>
+        <v>0.14159999787807465</v>
       </c>
       <c r="G32">
-        <v>0.16120000183582306</v>
+        <v>0.17949999868869781</v>
       </c>
       <c r="H32">
-        <v>0.26969999074935913</v>
+        <v>0.53030002117156982</v>
       </c>
       <c r="I32">
-        <v>0.27369999885559082</v>
+        <v>0.51800000667572021</v>
       </c>
       <c r="J32">
-        <v>0.25440001487731934</v>
+        <v>0.52340000867843628</v>
       </c>
       <c r="K32">
-        <v>8.529999852180481E-2</v>
-      </c>
-      <c r="L32">
-        <v>8.7300002574920654E-2</v>
-      </c>
-      <c r="M32">
-        <v>9.1600000858306885E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.11990000307559967</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B33">
-        <v>0.12919999659061432</v>
+        <v>0.13809999823570251</v>
       </c>
       <c r="C33">
-        <v>0.10130000114440918</v>
+        <v>0.1315000057220459</v>
       </c>
       <c r="D33">
-        <v>0.10109999775886536</v>
+        <v>0.13289999961853027</v>
       </c>
       <c r="E33">
-        <v>0.15530000627040863</v>
+        <v>2.461400032043457</v>
       </c>
       <c r="F33">
-        <v>0.1550000011920929</v>
+        <v>2.4158999919891357</v>
       </c>
       <c r="G33">
-        <v>0.15659999847412109</v>
+        <v>2.47760009765625</v>
       </c>
       <c r="H33">
-        <v>0.19310000538825989</v>
+        <v>0.37950000166893005</v>
       </c>
       <c r="I33">
-        <v>0.19529999792575836</v>
+        <v>0.33329999446868896</v>
       </c>
       <c r="J33">
-        <v>0.19140000641345978</v>
+        <v>0.34599998593330383</v>
       </c>
       <c r="K33">
-        <v>8.5600003600120544E-2</v>
-      </c>
-      <c r="L33">
-        <v>8.7300002574920654E-2</v>
-      </c>
-      <c r="M33">
-        <v>9.920000284910202E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.10480000078678131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B34">
-        <v>0.15729999542236328</v>
+        <v>0.17090000212192535</v>
       </c>
       <c r="C34">
-        <v>9.8099999129772186E-2</v>
+        <v>0.13750000298023224</v>
       </c>
       <c r="D34">
-        <v>9.6299998462200165E-2</v>
+        <v>0.13889999687671661</v>
       </c>
       <c r="E34">
-        <v>0.15150000154972076</v>
+        <v>2.1059999465942383</v>
       </c>
       <c r="F34">
-        <v>0.13729999959468842</v>
+        <v>2.0099000930786133</v>
       </c>
       <c r="G34">
-        <v>0.13689999282360077</v>
+        <v>1.9559999704360962</v>
       </c>
       <c r="H34">
-        <v>0.1664000004529953</v>
+        <v>0.23340000212192535</v>
       </c>
       <c r="I34">
-        <v>0.1648000031709671</v>
+        <v>0.2386000007390976</v>
       </c>
       <c r="J34">
-        <v>0.15610000491142273</v>
+        <v>0.23160000145435333</v>
       </c>
       <c r="K34">
-        <v>8.3800002932548523E-2</v>
-      </c>
-      <c r="L34">
-        <v>9.5100000500679016E-2</v>
-      </c>
-      <c r="M34">
-        <v>0.12880000472068787</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0.12200000137090683</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>

</xml_diff>